<commit_message>
Latest Commitbefore addition to logistics package.
</commit_message>
<xml_diff>
--- a/conf/coa.xlsx
+++ b/conf/coa.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="book_keeping" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -386,7 +387,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -398,14 +398,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -619,7 +617,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2318,11 +2316,37 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated account balance enquiry.
</commit_message>
<xml_diff>
--- a/conf/coa.xlsx
+++ b/conf/coa.xlsx
@@ -5,353 +5,361 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="book_keeping" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="112">
-  <si>
-    <t>Account Name</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Financial Statement</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Sub-Group</t>
-  </si>
-  <si>
-    <t>Normally</t>
-  </si>
-  <si>
-    <t>Bank checking account</t>
-  </si>
-  <si>
-    <t>Balance sheet</t>
-  </si>
-  <si>
-    <t>Current assets</t>
-  </si>
-  <si>
-    <t>Cash and cash equivalents</t>
-  </si>
-  <si>
-    <t>Debit</t>
-  </si>
-  <si>
-    <t>Bank savings account</t>
-  </si>
-  <si>
-    <t>Online savings account</t>
-  </si>
-  <si>
-    <t>Petty cash account</t>
-  </si>
-  <si>
-    <t>Paypal account</t>
-  </si>
-  <si>
-    <t>Accounts receivable</t>
-  </si>
-  <si>
-    <t>Allowance for doubtful debts account</t>
-  </si>
-  <si>
-    <t>Credit</t>
-  </si>
-  <si>
-    <t>Stock/Inventory</t>
-  </si>
-  <si>
-    <t>Inventory</t>
-  </si>
-  <si>
-    <t>Prepayments</t>
-  </si>
-  <si>
-    <t>Other current assets</t>
-  </si>
-  <si>
-    <t>Property</t>
-  </si>
-  <si>
-    <t>Long term assets</t>
-  </si>
-  <si>
-    <t>Property, plant and equipment</t>
-  </si>
-  <si>
-    <t>Property Depreciation</t>
-  </si>
-  <si>
-    <t>Plant</t>
-  </si>
-  <si>
-    <t>Plant depreciation</t>
-  </si>
-  <si>
-    <t>Equipment</t>
-  </si>
-  <si>
-    <t>Equipment depreciation</t>
-  </si>
-  <si>
-    <t>Accounts payable</t>
-  </si>
-  <si>
-    <t>Current liabilities</t>
-  </si>
-  <si>
-    <t>Payroll payable</t>
-  </si>
-  <si>
-    <t>Other current liabilities</t>
-  </si>
-  <si>
-    <t>Interest payable</t>
-  </si>
-  <si>
-    <t>Accrued expenses</t>
-  </si>
-  <si>
-    <t>Unearned revenue</t>
-  </si>
-  <si>
-    <t>Sales Tax payable</t>
-  </si>
-  <si>
-    <t>Purchase Tax payable</t>
-  </si>
-  <si>
-    <t>Payroll tax payable</t>
-  </si>
-  <si>
-    <t>Income tax payable</t>
-  </si>
-  <si>
-    <t>Mortgage loan</t>
-  </si>
-  <si>
-    <t>Long-term liabilities</t>
-  </si>
-  <si>
-    <t>Mortgages</t>
-  </si>
-  <si>
-    <t>Other loans</t>
-  </si>
-  <si>
-    <t>Loans</t>
-  </si>
-  <si>
-    <t>Owners contributions</t>
-  </si>
-  <si>
-    <t>Equity</t>
-  </si>
-  <si>
-    <t>Capital</t>
-  </si>
-  <si>
-    <t>Owners draw</t>
-  </si>
-  <si>
-    <t>Retained earnings</t>
-  </si>
-  <si>
-    <t>Retail sales</t>
-  </si>
-  <si>
-    <t>Income Statement</t>
-  </si>
-  <si>
-    <t>Income</t>
-  </si>
-  <si>
-    <t>Revenue</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>Discounts allowed</t>
-  </si>
-  <si>
-    <t>Purchases</t>
-  </si>
-  <si>
-    <t>Cost of sales</t>
-  </si>
-  <si>
-    <t>Packaging</t>
-  </si>
-  <si>
-    <t>Discounts taken</t>
-  </si>
-  <si>
-    <t>Shipping costs</t>
-  </si>
-  <si>
-    <t>Import duty</t>
-  </si>
-  <si>
-    <t>Opening stock/inventory</t>
-  </si>
-  <si>
-    <t>Closing stock/inventory</t>
-  </si>
-  <si>
-    <t>Productive Labour</t>
-  </si>
-  <si>
-    <t>Research and development</t>
-  </si>
-  <si>
-    <t>Expense</t>
-  </si>
-  <si>
-    <t>Sales commissions</t>
-  </si>
-  <si>
-    <t>Sales and marketing</t>
-  </si>
-  <si>
-    <t>Sales promotion</t>
-  </si>
-  <si>
-    <t>Advertising</t>
-  </si>
-  <si>
-    <t>Gifts &amp; samples</t>
-  </si>
-  <si>
-    <t>Marketing expenses</t>
-  </si>
-  <si>
-    <t>Payroll</t>
-  </si>
-  <si>
-    <t>General and administrative</t>
-  </si>
-  <si>
-    <t>Contract labor</t>
-  </si>
-  <si>
-    <t>Payroll expenses</t>
-  </si>
-  <si>
-    <t>Payroll benefits</t>
-  </si>
-  <si>
-    <t>Payroll taxes</t>
-  </si>
-  <si>
-    <t>Computer and internet</t>
-  </si>
-  <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Rent</t>
-  </si>
-  <si>
-    <t>Property taxes</t>
-  </si>
-  <si>
-    <t>Utilities</t>
-  </si>
-  <si>
-    <t>Motor expenses</t>
-  </si>
-  <si>
-    <t>Travelling</t>
-  </si>
-  <si>
-    <t>Hotels</t>
-  </si>
-  <si>
-    <t>Meals and entertainment</t>
-  </si>
-  <si>
-    <t>Printing</t>
-  </si>
-  <si>
-    <t>Postage &amp; carriage</t>
-  </si>
-  <si>
-    <t>Telephone</t>
-  </si>
-  <si>
-    <t>Office supplies</t>
-  </si>
-  <si>
-    <t>Professional fees</t>
-  </si>
-  <si>
-    <t>Equipment hire</t>
-  </si>
-  <si>
-    <t>Repairs &amp; maintenance</t>
-  </si>
-  <si>
-    <t>Housekeeping supplies and cleaning</t>
-  </si>
-  <si>
-    <t>Bad debt expense</t>
-  </si>
-  <si>
-    <t>Dues and membership fees</t>
-  </si>
-  <si>
-    <t>Research and professional development</t>
-  </si>
-  <si>
-    <t>Insurance</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>Suspense account</t>
-  </si>
-  <si>
-    <t>Depreciation</t>
-  </si>
-  <si>
-    <t>Interest expense</t>
-  </si>
-  <si>
-    <t>Finance costs</t>
-  </si>
-  <si>
-    <t>Bank fees</t>
-  </si>
-  <si>
-    <t>Interest income</t>
-  </si>
-  <si>
-    <t>Other Income</t>
-  </si>
-  <si>
-    <t>Rent income</t>
-  </si>
-  <si>
-    <t>Income tax expense</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="113">
+  <si>
+    <t xml:space="preserve">Account Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial Statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank checking account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash and cash equivalents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank savings account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online savings account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petty cash account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paypal account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts receivable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowance for doubtful debts account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock/Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepayments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other current assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long term assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property, plant and equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property Depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Payroll payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other current liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accrued expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unearned revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Tax payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Tax payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll tax payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income tax payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage loan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long-term liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owners contributions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owners draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retained earnings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income Statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discounts allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost of sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packaging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discounts taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shipping costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import duty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opening stock/inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closing stock/inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Productive Labour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research and development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales commissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales and marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advertising</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gifts &amp; samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketing expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General and administrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract labor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer and internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meals and entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postage &amp; carriage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment hire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repairs &amp; maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housekeeping supplies and cleaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad debt expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dues and membership fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research and professional development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspense account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rent income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income tax expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll payable</t>
   </si>
 </sst>
 </file>
@@ -359,13 +367,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -387,23 +396,27 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -489,9 +502,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -524,14 +539,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -544,7 +551,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Note" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Note" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -616,19 +623,19 @@
   </sheetPr>
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="58.6836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="29.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="40.5051020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="16.3775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="29.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="16.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -662,13 +669,13 @@
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="0"/>
@@ -683,13 +690,13 @@
       <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="0"/>
@@ -704,13 +711,13 @@
       <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="0"/>
@@ -725,13 +732,13 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="0"/>
@@ -746,13 +753,13 @@
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="0"/>
@@ -767,13 +774,13 @@
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="0"/>
@@ -788,13 +795,13 @@
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I8" s="0"/>
@@ -809,13 +816,13 @@
       <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="0"/>
@@ -830,13 +837,13 @@
       <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="0"/>
@@ -851,13 +858,13 @@
       <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I11" s="0"/>
@@ -872,13 +879,13 @@
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="0"/>
@@ -893,13 +900,13 @@
       <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I13" s="0"/>
@@ -914,13 +921,13 @@
       <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="0"/>
@@ -935,13 +942,13 @@
       <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I15" s="0"/>
@@ -956,13 +963,13 @@
       <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="0"/>
@@ -977,13 +984,13 @@
       <c r="C17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="0"/>
@@ -998,13 +1005,13 @@
       <c r="C18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I18" s="0"/>
@@ -1019,13 +1026,13 @@
       <c r="C19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="0"/>
@@ -1040,13 +1047,13 @@
       <c r="C20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="0"/>
@@ -1061,13 +1068,13 @@
       <c r="C21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I21" s="0"/>
@@ -1082,13 +1089,13 @@
       <c r="C22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I22" s="0"/>
@@ -1103,13 +1110,13 @@
       <c r="C23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I23" s="0"/>
@@ -1124,13 +1131,13 @@
       <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I24" s="0"/>
@@ -1145,13 +1152,13 @@
       <c r="C25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I25" s="0"/>
@@ -1166,13 +1173,13 @@
       <c r="C26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I26" s="0"/>
@@ -1187,13 +1194,13 @@
       <c r="C27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I27" s="0"/>
@@ -1208,13 +1215,13 @@
       <c r="C28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I28" s="0"/>
@@ -1229,13 +1236,13 @@
       <c r="C29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I29" s="0"/>
@@ -1250,13 +1257,13 @@
       <c r="C30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I30" s="0"/>
@@ -1271,13 +1278,13 @@
       <c r="C31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I31" s="0"/>
@@ -1292,13 +1299,13 @@
       <c r="C32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I32" s="0"/>
@@ -1313,13 +1320,13 @@
       <c r="C33" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I33" s="0"/>
@@ -1334,13 +1341,13 @@
       <c r="C34" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I34" s="0"/>
@@ -1355,13 +1362,13 @@
       <c r="C35" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I35" s="0"/>
@@ -1376,13 +1383,13 @@
       <c r="C36" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I36" s="0"/>
@@ -1397,13 +1404,13 @@
       <c r="C37" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I37" s="0"/>
@@ -1418,13 +1425,13 @@
       <c r="C38" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I38" s="0"/>
@@ -1439,13 +1446,13 @@
       <c r="C39" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I39" s="0"/>
@@ -1460,13 +1467,13 @@
       <c r="C40" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="7" t="s">
         <v>17</v>
       </c>
       <c r="I40" s="0"/>
@@ -1481,19 +1488,19 @@
       <c r="C41" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B42" s="7" t="n">
@@ -1502,13 +1509,13 @@
       <c r="C42" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="F42" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I42" s="0"/>
@@ -1523,16 +1530,16 @@
       <c r="C43" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I43" s="10"/>
+      <c r="F43" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
@@ -1544,13 +1551,13 @@
       <c r="C44" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1564,13 +1571,13 @@
       <c r="C45" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1584,13 +1591,13 @@
       <c r="C46" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1604,13 +1611,13 @@
       <c r="C47" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1624,13 +1631,13 @@
       <c r="C48" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1644,13 +1651,13 @@
       <c r="C49" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1664,13 +1671,13 @@
       <c r="C50" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1684,13 +1691,13 @@
       <c r="C51" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1704,13 +1711,13 @@
       <c r="C52" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1724,13 +1731,13 @@
       <c r="C53" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D53" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="F53" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1744,13 +1751,13 @@
       <c r="C54" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F54" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1764,13 +1771,13 @@
       <c r="C55" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="F55" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1784,13 +1791,13 @@
       <c r="C56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F56" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1804,13 +1811,13 @@
       <c r="C57" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1824,13 +1831,13 @@
       <c r="C58" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1844,13 +1851,13 @@
       <c r="C59" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F59" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1864,13 +1871,13 @@
       <c r="C60" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="F60" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1884,13 +1891,13 @@
       <c r="C61" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="F61" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1904,13 +1911,13 @@
       <c r="C62" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F62" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1924,13 +1931,13 @@
       <c r="C63" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D63" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="F63" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1944,13 +1951,13 @@
       <c r="C64" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="F64" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1964,13 +1971,13 @@
       <c r="C65" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D65" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F65" s="9" t="s">
+      <c r="F65" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1984,13 +1991,13 @@
       <c r="C66" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F66" s="9" t="s">
+      <c r="F66" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2004,13 +2011,13 @@
       <c r="C67" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="D67" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F67" s="9" t="s">
+      <c r="F67" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2024,13 +2031,13 @@
       <c r="C68" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="D68" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F68" s="9" t="s">
+      <c r="F68" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2044,13 +2051,13 @@
       <c r="C69" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="D69" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2064,13 +2071,13 @@
       <c r="C70" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2084,13 +2091,13 @@
       <c r="C71" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F71" s="9" t="s">
+      <c r="F71" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2104,13 +2111,13 @@
       <c r="C72" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D72" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F72" s="9" t="s">
+      <c r="F72" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2124,13 +2131,13 @@
       <c r="C73" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F73" s="9" t="s">
+      <c r="F73" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2144,13 +2151,13 @@
       <c r="C74" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="F74" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2164,13 +2171,13 @@
       <c r="C75" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F75" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2184,13 +2191,13 @@
       <c r="C76" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D76" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2204,13 +2211,13 @@
       <c r="C77" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="F77" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2224,13 +2231,13 @@
       <c r="C78" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="F78" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2244,13 +2251,13 @@
       <c r="C79" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="D79" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="F79" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2264,13 +2271,13 @@
       <c r="C80" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F80" s="9" t="s">
+      <c r="F80" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2284,13 +2291,13 @@
       <c r="C81" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F81" s="9" t="s">
+      <c r="F81" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2304,20 +2311,20 @@
       <c r="C82" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D82" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F82" s="9" t="s">
+      <c r="F82" s="7" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2330,20 +2337,1710 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="29.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="16.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>1010</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>1020</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>1030</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>1040</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>1210</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>1400</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>1600</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>1800</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>1810</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>1820</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="n">
+        <v>1830</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7" t="n">
+        <v>1840</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>1850</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>2200</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>2210</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>2220</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>2230</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="7" t="n">
+        <v>2240</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="7" t="n">
+        <v>2250</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="7" t="n">
+        <v>2260</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="7" t="n">
+        <v>2270</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="7" t="n">
+        <v>2400</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="7" t="n">
+        <v>2600</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="7" t="n">
+        <v>3010</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="7" t="n">
+        <v>3020</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="7" t="n">
+        <v>4000</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="7" t="n">
+        <v>4010</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="7" t="n">
+        <v>4020</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="7" t="n">
+        <v>4400</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="7" t="n">
+        <v>4410</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="7" t="n">
+        <v>4420</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="7" t="n">
+        <v>4430</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="7" t="n">
+        <v>4440</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="7" t="n">
+        <v>4450</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="7" t="n">
+        <v>4460</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="7" t="n">
+        <v>4470</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="7" t="n">
+        <v>4800</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="7" t="n">
+        <v>5010</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="7" t="n">
+        <v>5020</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="7" t="n">
+        <v>5030</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="7" t="n">
+        <v>5040</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="7" t="n">
+        <v>5200</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="7" t="n">
+        <v>5210</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="7" t="n">
+        <v>5220</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="7" t="n">
+        <v>5230</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="7" t="n">
+        <v>5240</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="7" t="n">
+        <v>5250</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="7" t="n">
+        <v>5260</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" s="7" t="n">
+        <v>5270</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="7" t="n">
+        <v>5280</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="7" t="n">
+        <v>5290</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="7" t="n">
+        <v>5300</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B59" s="7" t="n">
+        <v>5310</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="7" t="n">
+        <v>5320</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="7" t="n">
+        <v>5330</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="7" t="n">
+        <v>5340</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" s="7" t="n">
+        <v>5350</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" s="7" t="n">
+        <v>5360</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65" s="7" t="n">
+        <v>5370</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" s="7" t="n">
+        <v>5380</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="7" t="n">
+        <v>5390</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="7" t="n">
+        <v>5400</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B69" s="7" t="n">
+        <v>5410</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="7" t="n">
+        <v>5420</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71" s="7" t="n">
+        <v>5430</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72" s="7" t="n">
+        <v>5440</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="7" t="n">
+        <v>5450</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B74" s="7" t="n">
+        <v>5460</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B75" s="7" t="n">
+        <v>5470</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" s="7" t="n">
+        <v>5480</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" s="7" t="n">
+        <v>5600</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" s="7" t="n">
+        <v>5800</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B79" s="7" t="n">
+        <v>5810</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" s="7" t="n">
+        <v>4200</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" s="7" t="n">
+        <v>4210</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" s="7" t="n">
+        <v>5900</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Started working on a custom admin, accepted the fact that integrating bootstrap templates will be too much work, just write out the css from scratch.
</commit_message>
<xml_diff>
--- a/conf/coa.xlsx
+++ b/conf/coa.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="117">
   <si>
     <t xml:space="preserve">Account Name</t>
   </si>
@@ -41,21 +41,318 @@
     <t xml:space="preserve">Normally</t>
   </si>
   <si>
+    <t xml:space="preserve">Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash and cash equivalents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank Savings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petty Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts receivable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowance for bad debts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock/Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepayments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other current assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long term assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property, plant and equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property Depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plant depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other current liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accrued expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unearned revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Tax payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Tax payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll tax payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income tax payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgage loan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long-term liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mortgages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owners contributions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owners draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retained earnings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income Statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discounts allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost of sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packaging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discounts taken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shipping costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import duty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opening stock/inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closing stock/inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Productive Labour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research and development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales commissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales and marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advertising</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gifts &amp; samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketing expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General and administrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract labor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer and internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meals and entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postage &amp; carriage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment hire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repairs &amp; maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleaning supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad debt expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dues and membership fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspense account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rent income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income tax expense</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bank checking account</t>
   </si>
   <si>
-    <t xml:space="preserve">Balance sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cash and cash equivalents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bank savings account</t>
   </si>
   <si>
@@ -68,298 +365,13 @@
     <t xml:space="preserve">Paypal account</t>
   </si>
   <si>
-    <t xml:space="preserve">Accounts receivable</t>
-  </si>
-  <si>
     <t xml:space="preserve">Allowance for doubtful debts account</t>
   </si>
   <si>
-    <t xml:space="preserve">Credit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stock/Inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prepayments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other current assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long term assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property, plant and equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property Depreciation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plant depreciation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equipment depreciation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accounts payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current liabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Net Payroll payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other current liabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accrued expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unearned revenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales Tax payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase Tax payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll tax payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income tax payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgage loan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long-term liabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortgages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other loans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owners contributions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owners draw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retained earnings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail sales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income Statement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discounts allowed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost of sales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packaging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discounts taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shipping costs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Import duty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opening stock/inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closing stock/inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Productive Labour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research and development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales commissions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales and marketing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales promotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advertising</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gifts &amp; samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marketing expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General and administrative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contract labor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll benefits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll taxes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer and internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property taxes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travelling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hotels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meals and entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Printing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postage &amp; carriage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telephone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Office supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professional fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equipment hire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repairs &amp; maintenance</t>
-  </si>
-  <si>
     <t xml:space="preserve">Housekeeping supplies and cleaning</t>
   </si>
   <si>
-    <t xml:space="preserve">Bad debt expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dues and membership fees</t>
-  </si>
-  <si>
     <t xml:space="preserve">Research and professional development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suspense account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depreciation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance costs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rent income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income tax expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll payable</t>
   </si>
 </sst>
 </file>
@@ -551,7 +563,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Note" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -621,10 +633,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -706,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="7" t="n">
-        <v>1020</v>
+        <v>1030</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -727,7 +739,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="7" t="n">
-        <v>1030</v>
+        <v>1200</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>7</v>
@@ -736,7 +748,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>10</v>
@@ -748,7 +760,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="7" t="n">
-        <v>1040</v>
+        <v>1210</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>7</v>
@@ -757,19 +769,19 @@
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="7" t="n">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
@@ -778,7 +790,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>10</v>
@@ -787,10 +799,10 @@
     </row>
     <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7" t="n">
-        <v>1210</v>
+        <v>1600</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>7</v>
@@ -799,28 +811,28 @@
         <v>8</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="7" t="n">
-        <v>1400</v>
+        <v>1800</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>10</v>
@@ -829,40 +841,40 @@
     </row>
     <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B10" s="7" t="n">
-        <v>1600</v>
+        <v>1810</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>1820</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="7" t="n">
-        <v>1800</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>10</v>
@@ -874,19 +886,19 @@
         <v>25</v>
       </c>
       <c r="B12" s="7" t="n">
-        <v>1810</v>
+        <v>1830</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I12" s="0"/>
     </row>
@@ -895,16 +907,16 @@
         <v>26</v>
       </c>
       <c r="B13" s="7" t="n">
-        <v>1820</v>
+        <v>1840</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>10</v>
@@ -916,19 +928,19 @@
         <v>27</v>
       </c>
       <c r="B14" s="7" t="n">
-        <v>1830</v>
+        <v>1850</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I14" s="0"/>
     </row>
@@ -937,82 +949,82 @@
         <v>28</v>
       </c>
       <c r="B15" s="7" t="n">
-        <v>1840</v>
+        <v>2000</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>2200</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="7" t="n">
-        <v>1850</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B17" s="7" t="n">
-        <v>2000</v>
+        <v>2210</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="F17" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="7" t="n">
-        <v>2200</v>
+        <v>2220</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F18" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I18" s="0"/>
     </row>
@@ -1021,19 +1033,19 @@
         <v>34</v>
       </c>
       <c r="B19" s="7" t="n">
-        <v>2210</v>
+        <v>2230</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F19" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I19" s="0"/>
     </row>
@@ -1042,19 +1054,19 @@
         <v>35</v>
       </c>
       <c r="B20" s="7" t="n">
-        <v>2220</v>
+        <v>2240</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F20" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I20" s="0"/>
     </row>
@@ -1063,19 +1075,19 @@
         <v>36</v>
       </c>
       <c r="B21" s="7" t="n">
-        <v>2230</v>
+        <v>2250</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I21" s="0"/>
     </row>
@@ -1084,19 +1096,19 @@
         <v>37</v>
       </c>
       <c r="B22" s="7" t="n">
-        <v>2240</v>
+        <v>2260</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F22" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I22" s="0"/>
     </row>
@@ -1105,19 +1117,19 @@
         <v>38</v>
       </c>
       <c r="B23" s="7" t="n">
-        <v>2250</v>
+        <v>2270</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F23" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I23" s="0"/>
     </row>
@@ -1126,103 +1138,103 @@
         <v>39</v>
       </c>
       <c r="B24" s="7" t="n">
-        <v>2260</v>
+        <v>2400</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="7" t="n">
+        <v>2600</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="7" t="n">
-        <v>2270</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="E25" s="6" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B26" s="7" t="n">
-        <v>2400</v>
+        <v>3000</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B27" s="7" t="n">
-        <v>2600</v>
+        <v>3010</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B28" s="7" t="n">
-        <v>3000</v>
+        <v>3020</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I28" s="0"/>
     </row>
@@ -1231,61 +1243,61 @@
         <v>49</v>
       </c>
       <c r="B29" s="7" t="n">
-        <v>3010</v>
+        <v>4000</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B30" s="7" t="n">
-        <v>3020</v>
+        <v>4010</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="7" t="n">
+        <v>4020</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="7" t="n">
-        <v>4000</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="F31" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I31" s="0"/>
     </row>
@@ -1294,37 +1306,37 @@
         <v>55</v>
       </c>
       <c r="B32" s="7" t="n">
-        <v>4010</v>
+        <v>4400</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="7" t="n">
+        <v>4410</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="7" t="n">
-        <v>4020</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="E33" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>10</v>
@@ -1333,19 +1345,19 @@
     </row>
     <row r="34" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B34" s="7" t="n">
-        <v>4400</v>
+        <v>4420</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>10</v>
@@ -1357,16 +1369,16 @@
         <v>59</v>
       </c>
       <c r="B35" s="7" t="n">
-        <v>4410</v>
+        <v>4430</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>10</v>
@@ -1378,16 +1390,16 @@
         <v>60</v>
       </c>
       <c r="B36" s="7" t="n">
-        <v>4420</v>
+        <v>4440</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>10</v>
@@ -1399,16 +1411,16 @@
         <v>61</v>
       </c>
       <c r="B37" s="7" t="n">
-        <v>4430</v>
+        <v>4450</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>10</v>
@@ -1420,19 +1432,19 @@
         <v>62</v>
       </c>
       <c r="B38" s="7" t="n">
-        <v>4440</v>
+        <v>4460</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I38" s="0"/>
     </row>
@@ -1441,16 +1453,16 @@
         <v>63</v>
       </c>
       <c r="B39" s="7" t="n">
-        <v>4450</v>
+        <v>4470</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>10</v>
@@ -1462,100 +1474,98 @@
         <v>64</v>
       </c>
       <c r="B40" s="7" t="n">
-        <v>4460</v>
+        <v>4800</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B41" s="7" t="n">
-        <v>4470</v>
+        <v>5000</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I41" s="0"/>
+      <c r="I41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B42" s="7" t="n">
-        <v>4800</v>
+        <v>5010</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="F42" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B43" s="7" t="n">
-        <v>5000</v>
+        <v>5020</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D43" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="F43" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="7" t="n">
-        <v>5010</v>
+        <v>5030</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>10</v>
@@ -1566,16 +1576,16 @@
         <v>71</v>
       </c>
       <c r="B45" s="7" t="n">
-        <v>5020</v>
+        <v>5040</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D45" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>10</v>
@@ -1586,16 +1596,16 @@
         <v>72</v>
       </c>
       <c r="B46" s="7" t="n">
-        <v>5030</v>
+        <v>5200</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>10</v>
@@ -1603,19 +1613,19 @@
     </row>
     <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B47" s="7" t="n">
-        <v>5040</v>
+        <v>5210</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>10</v>
@@ -1623,19 +1633,19 @@
     </row>
     <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B48" s="7" t="n">
-        <v>5200</v>
+        <v>5220</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>10</v>
@@ -1646,16 +1656,16 @@
         <v>76</v>
       </c>
       <c r="B49" s="7" t="n">
-        <v>5210</v>
+        <v>5230</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>10</v>
@@ -1666,16 +1676,16 @@
         <v>77</v>
       </c>
       <c r="B50" s="7" t="n">
-        <v>5220</v>
+        <v>5240</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>10</v>
@@ -1686,16 +1696,16 @@
         <v>78</v>
       </c>
       <c r="B51" s="7" t="n">
-        <v>5230</v>
+        <v>5250</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>10</v>
@@ -1706,16 +1716,16 @@
         <v>79</v>
       </c>
       <c r="B52" s="7" t="n">
-        <v>5240</v>
+        <v>5260</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>10</v>
@@ -1726,16 +1736,16 @@
         <v>80</v>
       </c>
       <c r="B53" s="7" t="n">
-        <v>5250</v>
+        <v>5270</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>10</v>
@@ -1746,16 +1756,16 @@
         <v>81</v>
       </c>
       <c r="B54" s="7" t="n">
-        <v>5260</v>
+        <v>5280</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>10</v>
@@ -1766,16 +1776,16 @@
         <v>82</v>
       </c>
       <c r="B55" s="7" t="n">
-        <v>5270</v>
+        <v>5290</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>10</v>
@@ -1786,16 +1796,16 @@
         <v>83</v>
       </c>
       <c r="B56" s="7" t="n">
-        <v>5280</v>
+        <v>5300</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>10</v>
@@ -1806,16 +1816,16 @@
         <v>84</v>
       </c>
       <c r="B57" s="7" t="n">
-        <v>5290</v>
+        <v>5310</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>10</v>
@@ -1826,16 +1836,16 @@
         <v>85</v>
       </c>
       <c r="B58" s="7" t="n">
-        <v>5300</v>
+        <v>5320</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>10</v>
@@ -1846,16 +1856,16 @@
         <v>86</v>
       </c>
       <c r="B59" s="7" t="n">
-        <v>5310</v>
+        <v>5330</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>10</v>
@@ -1866,16 +1876,16 @@
         <v>87</v>
       </c>
       <c r="B60" s="7" t="n">
-        <v>5320</v>
+        <v>5340</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>10</v>
@@ -1886,16 +1896,16 @@
         <v>88</v>
       </c>
       <c r="B61" s="7" t="n">
-        <v>5330</v>
+        <v>5350</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>10</v>
@@ -1906,16 +1916,16 @@
         <v>89</v>
       </c>
       <c r="B62" s="7" t="n">
-        <v>5340</v>
+        <v>5360</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>10</v>
@@ -1926,16 +1936,16 @@
         <v>90</v>
       </c>
       <c r="B63" s="7" t="n">
-        <v>5350</v>
+        <v>5370</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>10</v>
@@ -1946,16 +1956,16 @@
         <v>91</v>
       </c>
       <c r="B64" s="7" t="n">
-        <v>5360</v>
+        <v>5380</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>10</v>
@@ -1966,16 +1976,16 @@
         <v>92</v>
       </c>
       <c r="B65" s="7" t="n">
-        <v>5370</v>
+        <v>5390</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>10</v>
@@ -1986,16 +1996,16 @@
         <v>93</v>
       </c>
       <c r="B66" s="7" t="n">
-        <v>5380</v>
+        <v>5400</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>10</v>
@@ -2006,16 +2016,16 @@
         <v>94</v>
       </c>
       <c r="B67" s="7" t="n">
-        <v>5390</v>
+        <v>5410</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>10</v>
@@ -2026,16 +2036,16 @@
         <v>95</v>
       </c>
       <c r="B68" s="7" t="n">
-        <v>5400</v>
+        <v>5420</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>10</v>
@@ -2046,16 +2056,16 @@
         <v>96</v>
       </c>
       <c r="B69" s="7" t="n">
-        <v>5410</v>
+        <v>5430</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>10</v>
@@ -2066,16 +2076,16 @@
         <v>97</v>
       </c>
       <c r="B70" s="7" t="n">
-        <v>5420</v>
+        <v>5440</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>10</v>
@@ -2086,16 +2096,16 @@
         <v>98</v>
       </c>
       <c r="B71" s="7" t="n">
-        <v>5430</v>
+        <v>5460</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>10</v>
@@ -2106,16 +2116,16 @@
         <v>99</v>
       </c>
       <c r="B72" s="7" t="n">
-        <v>5440</v>
+        <v>5470</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>10</v>
@@ -2126,16 +2136,16 @@
         <v>100</v>
       </c>
       <c r="B73" s="7" t="n">
-        <v>5450</v>
+        <v>5480</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>10</v>
@@ -2146,16 +2156,16 @@
         <v>101</v>
       </c>
       <c r="B74" s="7" t="n">
-        <v>5460</v>
+        <v>5600</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>10</v>
@@ -2166,16 +2176,16 @@
         <v>102</v>
       </c>
       <c r="B75" s="7" t="n">
-        <v>5470</v>
+        <v>5800</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>10</v>
@@ -2183,19 +2193,19 @@
     </row>
     <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B76" s="7" t="n">
+        <v>5810</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="B76" s="7" t="n">
-        <v>5480</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>10</v>
@@ -2203,121 +2213,61 @@
     </row>
     <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B77" s="7" t="n">
-        <v>5600</v>
+        <v>4200</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B78" s="7" t="n">
-        <v>5800</v>
+        <v>4210</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>106</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B79" s="7" t="n">
-        <v>5810</v>
+        <v>5900</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B80" s="7" t="n">
-        <v>4200</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B81" s="7" t="n">
-        <v>4210</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B82" s="7" t="n">
-        <v>5900</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F82" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2377,7 +2327,7 @@
     </row>
     <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1000</v>
@@ -2398,7 +2348,7 @@
     </row>
     <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1010</v>
@@ -2419,7 +2369,7 @@
     </row>
     <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>1020</v>
@@ -2440,7 +2390,7 @@
     </row>
     <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1030</v>
@@ -2461,7 +2411,7 @@
     </row>
     <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>1040</v>
@@ -2482,7 +2432,7 @@
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>1200</v>
@@ -2494,7 +2444,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>10</v>
@@ -2503,7 +2453,7 @@
     </row>
     <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>1210</v>
@@ -2515,16 +2465,16 @@
         <v>8</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>1400</v>
@@ -2536,7 +2486,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>10</v>
@@ -2545,7 +2495,7 @@
     </row>
     <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>1600</v>
@@ -2557,7 +2507,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>10</v>
@@ -2566,7 +2516,7 @@
     </row>
     <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>1800</v>
@@ -2575,10 +2525,10 @@
         <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>10</v>
@@ -2587,7 +2537,7 @@
     </row>
     <row r="12" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>1810</v>
@@ -2596,19 +2546,19 @@
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="7" t="n">
         <v>1820</v>
@@ -2617,10 +2567,10 @@
         <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>10</v>
@@ -2629,7 +2579,7 @@
     </row>
     <row r="14" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>1830</v>
@@ -2638,19 +2588,19 @@
         <v>7</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>1840</v>
@@ -2659,10 +2609,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>10</v>
@@ -2671,7 +2621,7 @@
     </row>
     <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>1850</v>
@@ -2680,19 +2630,19 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>2000</v>
@@ -2701,19 +2651,19 @@
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>2200</v>
@@ -2722,19 +2672,19 @@
         <v>7</v>
       </c>
       <c r="D18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F18" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>2210</v>
@@ -2743,19 +2693,19 @@
         <v>7</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F19" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>2220</v>
@@ -2764,19 +2714,19 @@
         <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F20" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="7" t="n">
         <v>2230</v>
@@ -2785,19 +2735,19 @@
         <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>2240</v>
@@ -2806,19 +2756,19 @@
         <v>7</v>
       </c>
       <c r="D22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F22" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="7" t="n">
         <v>2250</v>
@@ -2827,19 +2777,19 @@
         <v>7</v>
       </c>
       <c r="D23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F23" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>2260</v>
@@ -2848,19 +2798,19 @@
         <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F24" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>2270</v>
@@ -2869,19 +2819,19 @@
         <v>7</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="F25" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>2400</v>
@@ -2890,19 +2840,19 @@
         <v>7</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" s="7" t="n">
         <v>2600</v>
@@ -2911,19 +2861,19 @@
         <v>7</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="7" t="n">
         <v>3000</v>
@@ -2932,19 +2882,19 @@
         <v>7</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29" s="7" t="n">
         <v>3010</v>
@@ -2953,19 +2903,19 @@
         <v>7</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>3020</v>
@@ -2974,73 +2924,73 @@
         <v>7</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B31" s="7" t="n">
         <v>4000</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="F31" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B32" s="7" t="n">
         <v>4010</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="F32" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="7" t="n">
         <v>4020</v>
       </c>
       <c r="C33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>10</v>
@@ -3049,19 +2999,19 @@
     </row>
     <row r="34" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" s="7" t="n">
         <v>4400</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>10</v>
@@ -3070,19 +3020,19 @@
     </row>
     <row r="35" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B35" s="7" t="n">
         <v>4410</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>10</v>
@@ -3091,19 +3041,19 @@
     </row>
     <row r="36" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>4420</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>10</v>
@@ -3112,19 +3062,19 @@
     </row>
     <row r="37" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" s="7" t="n">
         <v>4430</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>10</v>
@@ -3133,19 +3083,19 @@
     </row>
     <row r="38" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>4440</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>10</v>
@@ -3154,19 +3104,19 @@
     </row>
     <row r="39" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B39" s="7" t="n">
         <v>4450</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>10</v>
@@ -3175,40 +3125,40 @@
     </row>
     <row r="40" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B40" s="7" t="n">
         <v>4460</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B41" s="7" t="n">
         <v>4470</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>10</v>
@@ -3217,19 +3167,19 @@
     </row>
     <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B42" s="7" t="n">
         <v>4800</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>10</v>
@@ -3238,19 +3188,19 @@
     </row>
     <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B43" s="7" t="n">
         <v>5000</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D43" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>10</v>
@@ -3259,19 +3209,19 @@
     </row>
     <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B44" s="7" t="n">
         <v>5010</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>10</v>
@@ -3279,19 +3229,19 @@
     </row>
     <row r="45" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B45" s="7" t="n">
         <v>5020</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D45" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>10</v>
@@ -3299,19 +3249,19 @@
     </row>
     <row r="46" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" s="7" t="n">
         <v>5030</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>10</v>
@@ -3319,19 +3269,19 @@
     </row>
     <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" s="7" t="n">
         <v>5040</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D47" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>10</v>
@@ -3339,19 +3289,19 @@
     </row>
     <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B48" s="7" t="n">
         <v>5200</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>10</v>
@@ -3359,19 +3309,19 @@
     </row>
     <row r="49" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B49" s="7" t="n">
         <v>5210</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>10</v>
@@ -3379,19 +3329,19 @@
     </row>
     <row r="50" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B50" s="7" t="n">
         <v>5220</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>10</v>
@@ -3399,19 +3349,19 @@
     </row>
     <row r="51" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B51" s="7" t="n">
         <v>5230</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>10</v>
@@ -3419,19 +3369,19 @@
     </row>
     <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B52" s="7" t="n">
         <v>5240</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>10</v>
@@ -3439,19 +3389,19 @@
     </row>
     <row r="53" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B53" s="7" t="n">
         <v>5250</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>10</v>
@@ -3459,19 +3409,19 @@
     </row>
     <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B54" s="7" t="n">
         <v>5260</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>10</v>
@@ -3479,19 +3429,19 @@
     </row>
     <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B55" s="7" t="n">
         <v>5270</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>10</v>
@@ -3499,19 +3449,19 @@
     </row>
     <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B56" s="7" t="n">
         <v>5280</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>10</v>
@@ -3519,19 +3469,19 @@
     </row>
     <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B57" s="7" t="n">
         <v>5290</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>10</v>
@@ -3539,19 +3489,19 @@
     </row>
     <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B58" s="7" t="n">
         <v>5300</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>10</v>
@@ -3559,19 +3509,19 @@
     </row>
     <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B59" s="7" t="n">
         <v>5310</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>10</v>
@@ -3579,19 +3529,19 @@
     </row>
     <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B60" s="7" t="n">
         <v>5320</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>10</v>
@@ -3599,19 +3549,19 @@
     </row>
     <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B61" s="7" t="n">
         <v>5330</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>10</v>
@@ -3619,19 +3569,19 @@
     </row>
     <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B62" s="7" t="n">
         <v>5340</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>10</v>
@@ -3639,19 +3589,19 @@
     </row>
     <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B63" s="7" t="n">
         <v>5350</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>10</v>
@@ -3659,19 +3609,19 @@
     </row>
     <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B64" s="7" t="n">
         <v>5360</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>10</v>
@@ -3679,19 +3629,19 @@
     </row>
     <row r="65" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B65" s="7" t="n">
         <v>5370</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>10</v>
@@ -3699,19 +3649,19 @@
     </row>
     <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B66" s="7" t="n">
         <v>5380</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>10</v>
@@ -3719,19 +3669,19 @@
     </row>
     <row r="67" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B67" s="7" t="n">
         <v>5390</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>10</v>
@@ -3739,19 +3689,19 @@
     </row>
     <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B68" s="7" t="n">
         <v>5400</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>10</v>
@@ -3759,19 +3709,19 @@
     </row>
     <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B69" s="7" t="n">
         <v>5410</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>10</v>
@@ -3779,19 +3729,19 @@
     </row>
     <row r="70" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B70" s="7" t="n">
         <v>5420</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>10</v>
@@ -3799,19 +3749,19 @@
     </row>
     <row r="71" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B71" s="7" t="n">
         <v>5430</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>10</v>
@@ -3819,19 +3769,19 @@
     </row>
     <row r="72" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B72" s="7" t="n">
         <v>5440</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>10</v>
@@ -3839,19 +3789,19 @@
     </row>
     <row r="73" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B73" s="7" t="n">
         <v>5450</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>10</v>
@@ -3859,19 +3809,19 @@
     </row>
     <row r="74" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B74" s="7" t="n">
         <v>5460</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>10</v>
@@ -3879,19 +3829,19 @@
     </row>
     <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B75" s="7" t="n">
         <v>5470</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>10</v>
@@ -3899,19 +3849,19 @@
     </row>
     <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B76" s="7" t="n">
         <v>5480</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>10</v>
@@ -3919,19 +3869,19 @@
     </row>
     <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B77" s="7" t="n">
         <v>5600</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>10</v>
@@ -3939,19 +3889,19 @@
     </row>
     <row r="78" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B78" s="7" t="n">
         <v>5800</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>10</v>
@@ -3959,19 +3909,19 @@
     </row>
     <row r="79" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B79" s="7" t="n">
         <v>5810</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>10</v>
@@ -3979,59 +3929,59 @@
     </row>
     <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B80" s="7" t="n">
         <v>4200</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B81" s="7" t="n">
         <v>4210</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B82" s="7" t="n">
         <v>5900</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updates to make the app integrate better, specifically adding default settings.
</commit_message>
<xml_diff>
--- a/conf/coa.xlsx
+++ b/conf/coa.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="120">
   <si>
     <t xml:space="preserve">Account Name</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t xml:space="preserve">Debit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EcoCash</t>
   </si>
   <si>
     <t xml:space="preserve">Bank Savings</t>
@@ -636,10 +642,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B9" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9:D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -700,7 +706,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="7" t="n">
-        <v>1010</v>
+        <v>1001</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>7</v>
@@ -721,7 +727,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="7" t="n">
-        <v>1030</v>
+        <v>1002</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -742,7 +748,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="7" t="n">
-        <v>1200</v>
+        <v>1010</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>7</v>
@@ -751,7 +757,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>10</v>
@@ -763,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="7" t="n">
-        <v>1210</v>
+        <v>1030</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>7</v>
@@ -772,19 +778,19 @@
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7" t="n">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>7</v>
@@ -793,7 +799,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>10</v>
@@ -802,10 +808,10 @@
     </row>
     <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7" t="n">
-        <v>1600</v>
+        <v>1210</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>7</v>
@@ -814,28 +820,28 @@
         <v>8</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="7" t="n">
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>10</v>
@@ -844,40 +850,40 @@
     </row>
     <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7" t="n">
-        <v>1810</v>
+        <v>1600</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="F10" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>1800</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="7" t="n">
-        <v>1820</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>10</v>
@@ -889,19 +895,19 @@
         <v>25</v>
       </c>
       <c r="B12" s="7" t="n">
-        <v>1830</v>
+        <v>1810</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I12" s="0"/>
     </row>
@@ -910,16 +916,16 @@
         <v>26</v>
       </c>
       <c r="B13" s="7" t="n">
-        <v>1840</v>
+        <v>1820</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>10</v>
@@ -931,19 +937,19 @@
         <v>27</v>
       </c>
       <c r="B14" s="7" t="n">
-        <v>1850</v>
+        <v>1830</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I14" s="0"/>
     </row>
@@ -952,82 +958,82 @@
         <v>28</v>
       </c>
       <c r="B15" s="7" t="n">
-        <v>2000</v>
+        <v>1840</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7" t="n">
-        <v>2200</v>
+        <v>1850</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="7" t="n">
-        <v>2210</v>
+        <v>2000</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>2200</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="7" t="n">
-        <v>2220</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="F18" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I18" s="0"/>
     </row>
@@ -1036,19 +1042,19 @@
         <v>34</v>
       </c>
       <c r="B19" s="7" t="n">
-        <v>2230</v>
+        <v>2210</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I19" s="0"/>
     </row>
@@ -1057,19 +1063,19 @@
         <v>35</v>
       </c>
       <c r="B20" s="7" t="n">
-        <v>2240</v>
+        <v>2220</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I20" s="0"/>
     </row>
@@ -1078,19 +1084,19 @@
         <v>36</v>
       </c>
       <c r="B21" s="7" t="n">
-        <v>2250</v>
+        <v>2230</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I21" s="0"/>
     </row>
@@ -1099,19 +1105,19 @@
         <v>37</v>
       </c>
       <c r="B22" s="7" t="n">
-        <v>2260</v>
+        <v>2240</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I22" s="0"/>
     </row>
@@ -1120,19 +1126,19 @@
         <v>38</v>
       </c>
       <c r="B23" s="7" t="n">
-        <v>2270</v>
+        <v>2250</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I23" s="0"/>
     </row>
@@ -1141,103 +1147,103 @@
         <v>39</v>
       </c>
       <c r="B24" s="7" t="n">
-        <v>2400</v>
+        <v>2260</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="7" t="n">
-        <v>2600</v>
+        <v>2270</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B26" s="7" t="n">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B27" s="7" t="n">
-        <v>3010</v>
+        <v>2600</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="F27" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B28" s="7" t="n">
-        <v>3020</v>
+        <v>3000</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I28" s="0"/>
     </row>
@@ -1246,61 +1252,61 @@
         <v>49</v>
       </c>
       <c r="B29" s="7" t="n">
-        <v>4000</v>
+        <v>3010</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B30" s="7" t="n">
-        <v>4010</v>
+        <v>3020</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="F30" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="7" t="n">
+        <v>4000</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="7" t="n">
-        <v>4020</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="F31" s="7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I31" s="0"/>
     </row>
@@ -1309,37 +1315,37 @@
         <v>55</v>
       </c>
       <c r="B32" s="7" t="n">
-        <v>4400</v>
+        <v>4010</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" s="7" t="n">
-        <v>4410</v>
+        <v>4020</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>10</v>
@@ -1348,19 +1354,19 @@
     </row>
     <row r="34" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="7" t="n">
+        <v>4400</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="7" t="n">
-        <v>4420</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="E34" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>10</v>
@@ -1372,16 +1378,16 @@
         <v>59</v>
       </c>
       <c r="B35" s="7" t="n">
-        <v>4430</v>
+        <v>4410</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>10</v>
@@ -1393,16 +1399,16 @@
         <v>60</v>
       </c>
       <c r="B36" s="7" t="n">
-        <v>4440</v>
+        <v>4420</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>10</v>
@@ -1414,16 +1420,16 @@
         <v>61</v>
       </c>
       <c r="B37" s="7" t="n">
-        <v>4450</v>
+        <v>4430</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>10</v>
@@ -1435,19 +1441,19 @@
         <v>62</v>
       </c>
       <c r="B38" s="7" t="n">
-        <v>4460</v>
+        <v>4440</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I38" s="0"/>
     </row>
@@ -1456,16 +1462,16 @@
         <v>63</v>
       </c>
       <c r="B39" s="7" t="n">
-        <v>4470</v>
+        <v>4450</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>10</v>
@@ -1477,98 +1483,100 @@
         <v>64</v>
       </c>
       <c r="B40" s="7" t="n">
-        <v>4800</v>
+        <v>4460</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B41" s="7" t="n">
-        <v>5000</v>
+        <v>4470</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I41" s="8"/>
+      <c r="I41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B42" s="7" t="n">
-        <v>5010</v>
+        <v>4800</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="I42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="7" t="n">
-        <v>5020</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="F43" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="I43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="7" t="n">
-        <v>5030</v>
+        <v>5010</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>10</v>
@@ -1579,16 +1587,16 @@
         <v>71</v>
       </c>
       <c r="B45" s="7" t="n">
-        <v>5040</v>
+        <v>5020</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>10</v>
@@ -1599,16 +1607,16 @@
         <v>72</v>
       </c>
       <c r="B46" s="7" t="n">
-        <v>5200</v>
+        <v>5030</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>10</v>
@@ -1616,19 +1624,19 @@
     </row>
     <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" s="7" t="n">
-        <v>5210</v>
+        <v>5040</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>10</v>
@@ -1636,19 +1644,19 @@
     </row>
     <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="7" t="n">
-        <v>5220</v>
+        <v>5200</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>10</v>
@@ -1659,16 +1667,16 @@
         <v>76</v>
       </c>
       <c r="B49" s="7" t="n">
-        <v>5230</v>
+        <v>5210</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>10</v>
@@ -1679,16 +1687,16 @@
         <v>77</v>
       </c>
       <c r="B50" s="7" t="n">
-        <v>5240</v>
+        <v>5220</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>10</v>
@@ -1699,16 +1707,16 @@
         <v>78</v>
       </c>
       <c r="B51" s="7" t="n">
-        <v>5250</v>
+        <v>5230</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>10</v>
@@ -1719,16 +1727,16 @@
         <v>79</v>
       </c>
       <c r="B52" s="7" t="n">
-        <v>5260</v>
+        <v>5240</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>10</v>
@@ -1739,16 +1747,16 @@
         <v>80</v>
       </c>
       <c r="B53" s="7" t="n">
-        <v>5270</v>
+        <v>5250</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>10</v>
@@ -1759,16 +1767,16 @@
         <v>81</v>
       </c>
       <c r="B54" s="7" t="n">
-        <v>5280</v>
+        <v>5260</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>10</v>
@@ -1779,16 +1787,16 @@
         <v>82</v>
       </c>
       <c r="B55" s="7" t="n">
-        <v>5290</v>
+        <v>5270</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>10</v>
@@ -1799,16 +1807,16 @@
         <v>83</v>
       </c>
       <c r="B56" s="7" t="n">
-        <v>5300</v>
+        <v>5280</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>10</v>
@@ -1819,16 +1827,16 @@
         <v>84</v>
       </c>
       <c r="B57" s="7" t="n">
-        <v>5310</v>
+        <v>5290</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>10</v>
@@ -1839,16 +1847,16 @@
         <v>85</v>
       </c>
       <c r="B58" s="7" t="n">
-        <v>5320</v>
+        <v>5300</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>10</v>
@@ -1859,16 +1867,16 @@
         <v>86</v>
       </c>
       <c r="B59" s="7" t="n">
-        <v>5330</v>
+        <v>5310</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>10</v>
@@ -1879,16 +1887,16 @@
         <v>87</v>
       </c>
       <c r="B60" s="7" t="n">
-        <v>5340</v>
+        <v>5320</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>10</v>
@@ -1899,16 +1907,16 @@
         <v>88</v>
       </c>
       <c r="B61" s="7" t="n">
-        <v>5350</v>
+        <v>5330</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>10</v>
@@ -1919,16 +1927,16 @@
         <v>89</v>
       </c>
       <c r="B62" s="7" t="n">
-        <v>5360</v>
+        <v>5340</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>10</v>
@@ -1939,16 +1947,16 @@
         <v>90</v>
       </c>
       <c r="B63" s="7" t="n">
-        <v>5370</v>
+        <v>5350</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>10</v>
@@ -1959,16 +1967,16 @@
         <v>91</v>
       </c>
       <c r="B64" s="7" t="n">
-        <v>5380</v>
+        <v>5360</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>10</v>
@@ -1979,16 +1987,16 @@
         <v>92</v>
       </c>
       <c r="B65" s="7" t="n">
-        <v>5390</v>
+        <v>5370</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>10</v>
@@ -1999,16 +2007,16 @@
         <v>93</v>
       </c>
       <c r="B66" s="7" t="n">
-        <v>5400</v>
+        <v>5380</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>10</v>
@@ -2019,16 +2027,16 @@
         <v>94</v>
       </c>
       <c r="B67" s="7" t="n">
-        <v>5410</v>
+        <v>5390</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>10</v>
@@ -2039,16 +2047,16 @@
         <v>95</v>
       </c>
       <c r="B68" s="7" t="n">
-        <v>5420</v>
+        <v>5400</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>10</v>
@@ -2059,16 +2067,16 @@
         <v>96</v>
       </c>
       <c r="B69" s="7" t="n">
-        <v>5430</v>
+        <v>5410</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>10</v>
@@ -2079,16 +2087,16 @@
         <v>97</v>
       </c>
       <c r="B70" s="7" t="n">
-        <v>5440</v>
+        <v>5420</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>10</v>
@@ -2099,16 +2107,16 @@
         <v>98</v>
       </c>
       <c r="B71" s="7" t="n">
-        <v>5460</v>
+        <v>5430</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>10</v>
@@ -2119,16 +2127,16 @@
         <v>99</v>
       </c>
       <c r="B72" s="7" t="n">
-        <v>5470</v>
+        <v>5440</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>10</v>
@@ -2139,16 +2147,16 @@
         <v>100</v>
       </c>
       <c r="B73" s="7" t="n">
-        <v>5480</v>
+        <v>5460</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>10</v>
@@ -2159,16 +2167,16 @@
         <v>101</v>
       </c>
       <c r="B74" s="7" t="n">
-        <v>5600</v>
+        <v>5470</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>10</v>
@@ -2179,16 +2187,16 @@
         <v>102</v>
       </c>
       <c r="B75" s="7" t="n">
-        <v>5800</v>
+        <v>5480</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>10</v>
@@ -2196,16 +2204,16 @@
     </row>
     <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B76" s="7" t="n">
-        <v>5810</v>
+        <v>5600</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>103</v>
@@ -2216,61 +2224,101 @@
     </row>
     <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B77" s="7" t="n">
+        <v>5800</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B77" s="7" t="n">
-        <v>4200</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>106</v>
-      </c>
       <c r="F77" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B78" s="7" t="n">
-        <v>4210</v>
+        <v>5810</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B79" s="7" t="n">
-        <v>5900</v>
+        <v>4200</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>108</v>
       </c>
       <c r="F79" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B80" s="7" t="n">
+        <v>4210</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" s="7" t="n">
+        <v>5900</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2293,7 +2341,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="D9:D14 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2330,7 +2378,7 @@
     </row>
     <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1000</v>
@@ -2351,7 +2399,7 @@
     </row>
     <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1010</v>
@@ -2372,7 +2420,7 @@
     </row>
     <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>1020</v>
@@ -2393,7 +2441,7 @@
     </row>
     <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1030</v>
@@ -2414,7 +2462,7 @@
     </row>
     <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>1040</v>
@@ -2435,7 +2483,7 @@
     </row>
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>1200</v>
@@ -2447,7 +2495,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>10</v>
@@ -2456,7 +2504,7 @@
     </row>
     <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>1210</v>
@@ -2468,16 +2516,16 @@
         <v>8</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>1400</v>
@@ -2489,7 +2537,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>10</v>
@@ -2498,7 +2546,7 @@
     </row>
     <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>1600</v>
@@ -2510,7 +2558,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>10</v>
@@ -2519,7 +2567,7 @@
     </row>
     <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>1800</v>
@@ -2528,10 +2576,10 @@
         <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>10</v>
@@ -2540,7 +2588,7 @@
     </row>
     <row r="12" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>1810</v>
@@ -2549,19 +2597,19 @@
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" s="7" t="n">
         <v>1820</v>
@@ -2570,10 +2618,10 @@
         <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>10</v>
@@ -2582,7 +2630,7 @@
     </row>
     <row r="14" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>1830</v>
@@ -2591,19 +2639,19 @@
         <v>7</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>1840</v>
@@ -2612,10 +2660,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>10</v>
@@ -2624,7 +2672,7 @@
     </row>
     <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>1850</v>
@@ -2633,19 +2681,19 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>2000</v>
@@ -2654,19 +2702,19 @@
         <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>2200</v>
@@ -2675,19 +2723,19 @@
         <v>7</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>2210</v>
@@ -2696,19 +2744,19 @@
         <v>7</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>2220</v>
@@ -2717,19 +2765,19 @@
         <v>7</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="7" t="n">
         <v>2230</v>
@@ -2738,19 +2786,19 @@
         <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>2240</v>
@@ -2759,19 +2807,19 @@
         <v>7</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B23" s="7" t="n">
         <v>2250</v>
@@ -2780,19 +2828,19 @@
         <v>7</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>2260</v>
@@ -2801,19 +2849,19 @@
         <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>2270</v>
@@ -2822,19 +2870,19 @@
         <v>7</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>2400</v>
@@ -2843,19 +2891,19 @@
         <v>7</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B27" s="7" t="n">
         <v>2600</v>
@@ -2864,19 +2912,19 @@
         <v>7</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B28" s="7" t="n">
         <v>3000</v>
@@ -2885,19 +2933,19 @@
         <v>7</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B29" s="7" t="n">
         <v>3010</v>
@@ -2906,19 +2954,19 @@
         <v>7</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>3020</v>
@@ -2927,73 +2975,73 @@
         <v>7</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B31" s="7" t="n">
         <v>4000</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B32" s="7" t="n">
         <v>4010</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B33" s="7" t="n">
         <v>4020</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>10</v>
@@ -3002,19 +3050,19 @@
     </row>
     <row r="34" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B34" s="7" t="n">
         <v>4400</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>10</v>
@@ -3023,19 +3071,19 @@
     </row>
     <row r="35" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B35" s="7" t="n">
         <v>4410</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>10</v>
@@ -3044,19 +3092,19 @@
     </row>
     <row r="36" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>4420</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>10</v>
@@ -3065,19 +3113,19 @@
     </row>
     <row r="37" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B37" s="7" t="n">
         <v>4430</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>10</v>
@@ -3086,19 +3134,19 @@
     </row>
     <row r="38" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>4440</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>10</v>
@@ -3107,19 +3155,19 @@
     </row>
     <row r="39" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B39" s="7" t="n">
         <v>4450</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>10</v>
@@ -3128,40 +3176,40 @@
     </row>
     <row r="40" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B40" s="7" t="n">
         <v>4460</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B41" s="7" t="n">
         <v>4470</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>10</v>
@@ -3170,19 +3218,19 @@
     </row>
     <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B42" s="7" t="n">
         <v>4800</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>10</v>
@@ -3191,19 +3239,19 @@
     </row>
     <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B43" s="7" t="n">
         <v>5000</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>10</v>
@@ -3212,19 +3260,19 @@
     </row>
     <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B44" s="7" t="n">
         <v>5010</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>10</v>
@@ -3232,19 +3280,19 @@
     </row>
     <row r="45" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B45" s="7" t="n">
         <v>5020</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>10</v>
@@ -3252,19 +3300,19 @@
     </row>
     <row r="46" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B46" s="7" t="n">
         <v>5030</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>10</v>
@@ -3272,19 +3320,19 @@
     </row>
     <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B47" s="7" t="n">
         <v>5040</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>10</v>
@@ -3292,19 +3340,19 @@
     </row>
     <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B48" s="7" t="n">
         <v>5200</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>10</v>
@@ -3312,19 +3360,19 @@
     </row>
     <row r="49" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B49" s="7" t="n">
         <v>5210</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>10</v>
@@ -3332,19 +3380,19 @@
     </row>
     <row r="50" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B50" s="7" t="n">
         <v>5220</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>10</v>
@@ -3352,19 +3400,19 @@
     </row>
     <row r="51" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B51" s="7" t="n">
         <v>5230</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>10</v>
@@ -3372,19 +3420,19 @@
     </row>
     <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B52" s="7" t="n">
         <v>5240</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>10</v>
@@ -3392,19 +3440,19 @@
     </row>
     <row r="53" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B53" s="7" t="n">
         <v>5250</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>10</v>
@@ -3412,19 +3460,19 @@
     </row>
     <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B54" s="7" t="n">
         <v>5260</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>10</v>
@@ -3432,19 +3480,19 @@
     </row>
     <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B55" s="7" t="n">
         <v>5270</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>10</v>
@@ -3452,19 +3500,19 @@
     </row>
     <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B56" s="7" t="n">
         <v>5280</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>10</v>
@@ -3472,19 +3520,19 @@
     </row>
     <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B57" s="7" t="n">
         <v>5290</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>10</v>
@@ -3492,19 +3540,19 @@
     </row>
     <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B58" s="7" t="n">
         <v>5300</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>10</v>
@@ -3512,19 +3560,19 @@
     </row>
     <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B59" s="7" t="n">
         <v>5310</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>10</v>
@@ -3532,19 +3580,19 @@
     </row>
     <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B60" s="7" t="n">
         <v>5320</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>10</v>
@@ -3552,19 +3600,19 @@
     </row>
     <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B61" s="7" t="n">
         <v>5330</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>10</v>
@@ -3572,19 +3620,19 @@
     </row>
     <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B62" s="7" t="n">
         <v>5340</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>10</v>
@@ -3592,19 +3640,19 @@
     </row>
     <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B63" s="7" t="n">
         <v>5350</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>10</v>
@@ -3612,19 +3660,19 @@
     </row>
     <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B64" s="7" t="n">
         <v>5360</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>10</v>
@@ -3632,19 +3680,19 @@
     </row>
     <row r="65" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B65" s="7" t="n">
         <v>5370</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>10</v>
@@ -3652,19 +3700,19 @@
     </row>
     <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B66" s="7" t="n">
         <v>5380</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>10</v>
@@ -3672,19 +3720,19 @@
     </row>
     <row r="67" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B67" s="7" t="n">
         <v>5390</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>10</v>
@@ -3692,19 +3740,19 @@
     </row>
     <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B68" s="7" t="n">
         <v>5400</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>10</v>
@@ -3712,19 +3760,19 @@
     </row>
     <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B69" s="7" t="n">
         <v>5410</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>10</v>
@@ -3732,19 +3780,19 @@
     </row>
     <row r="70" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B70" s="7" t="n">
         <v>5420</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>10</v>
@@ -3752,19 +3800,19 @@
     </row>
     <row r="71" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B71" s="7" t="n">
         <v>5430</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>10</v>
@@ -3772,19 +3820,19 @@
     </row>
     <row r="72" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B72" s="7" t="n">
         <v>5440</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>10</v>
@@ -3792,19 +3840,19 @@
     </row>
     <row r="73" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B73" s="7" t="n">
         <v>5450</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>10</v>
@@ -3812,19 +3860,19 @@
     </row>
     <row r="74" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B74" s="7" t="n">
         <v>5460</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>10</v>
@@ -3832,19 +3880,19 @@
     </row>
     <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B75" s="7" t="n">
         <v>5470</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>10</v>
@@ -3852,19 +3900,19 @@
     </row>
     <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B76" s="7" t="n">
         <v>5480</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>10</v>
@@ -3872,19 +3920,19 @@
     </row>
     <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B77" s="7" t="n">
         <v>5600</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>10</v>
@@ -3892,19 +3940,19 @@
     </row>
     <row r="78" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B78" s="7" t="n">
         <v>5800</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>10</v>
@@ -3912,19 +3960,19 @@
     </row>
     <row r="79" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B79" s="7" t="n">
         <v>5810</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>10</v>
@@ -3932,59 +3980,59 @@
     </row>
     <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B80" s="7" t="n">
         <v>4200</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B81" s="7" t="n">
         <v>4210</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B82" s="7" t="n">
         <v>5900</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Included the capturing of more detailed information like receipt files.
</commit_message>
<xml_diff>
--- a/conf/coa.xlsx
+++ b/conf/coa.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="127">
   <si>
     <t xml:space="preserve">Account Name</t>
   </si>
@@ -218,163 +218,184 @@
     <t xml:space="preserve">Closing stock/inventory</t>
   </si>
   <si>
+    <t xml:space="preserve">Direct Labour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost of production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct Materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct Expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indirect Manufacturing Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indirect Labour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research and development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales commissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales and marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advertising</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gifts &amp; samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketing expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General and administrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract labor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payroll taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer and internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property taxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meals and entertainment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postage &amp; carriage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Professional fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment hire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repairs &amp; maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleaning supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad debt expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dues and membership fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspense account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank fees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rent income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income tax expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank checking account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank savings account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Online savings account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petty cash account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paypal account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowance for doubtful debts account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long term assets</t>
+  </si>
+  <si>
     <t xml:space="preserve">Productive Labour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research and development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales commissions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales and marketing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales promotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advertising</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gifts &amp; samples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marketing expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General and administrative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contract labor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll benefits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payroll taxes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer and internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property taxes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travelling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hotels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meals and entertainment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Printing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postage &amp; carriage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telephone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Office supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professional fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equipment hire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repairs &amp; maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cleaning supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bad debt expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dues and membership fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suspense account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depreciation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance costs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank fees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rent income</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income tax expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank checking account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank savings account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Online savings account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petty cash account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paypal account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allowance for doubtful debts account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long term assets</t>
   </si>
   <si>
     <t xml:space="preserve">Housekeeping supplies and cleaning</t>
@@ -390,7 +411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -429,6 +450,19 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -527,7 +561,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -560,7 +594,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -642,10 +688,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C34" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="41:46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1499,7 +1545,7 @@
       </c>
       <c r="I40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" s="9" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
         <v>65</v>
       </c>
@@ -1512,26 +1558,26 @@
       <c r="D41" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" s="9" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="7" t="n">
+        <v>4480</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="7" t="n">
-        <v>4800</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>66</v>
@@ -1539,121 +1585,125 @@
       <c r="F42" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" s="9" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B43" s="7" t="n">
-        <v>5000</v>
+        <v>4490</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E43" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" s="9" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I43" s="8"/>
-    </row>
-    <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
+      <c r="B44" s="7" t="n">
+        <v>4500</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="10"/>
+    </row>
+    <row r="45" s="9" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="7" t="n">
-        <v>5010</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="s">
+      <c r="B45" s="7" t="n">
+        <v>4510</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I45" s="10"/>
+    </row>
+    <row r="46" s="9" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="7" t="n">
-        <v>5020</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
-        <v>72</v>
-      </c>
       <c r="B46" s="7" t="n">
-        <v>5030</v>
+        <v>4520</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="I46" s="10"/>
     </row>
     <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="7" t="n">
-        <v>5040</v>
+        <v>4800</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="I47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B48" s="7" t="n">
-        <v>5200</v>
+        <v>5000</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>75</v>
@@ -1661,19 +1711,20 @@
       <c r="F48" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="I48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
         <v>76</v>
       </c>
       <c r="B49" s="7" t="n">
-        <v>5210</v>
+        <v>5010</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>75</v>
@@ -1687,13 +1738,13 @@
         <v>77</v>
       </c>
       <c r="B50" s="7" t="n">
-        <v>5220</v>
+        <v>5020</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>75</v>
@@ -1707,13 +1758,13 @@
         <v>78</v>
       </c>
       <c r="B51" s="7" t="n">
-        <v>5230</v>
+        <v>5030</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>75</v>
@@ -1727,13 +1778,13 @@
         <v>79</v>
       </c>
       <c r="B52" s="7" t="n">
-        <v>5240</v>
+        <v>5040</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>75</v>
@@ -1747,16 +1798,16 @@
         <v>80</v>
       </c>
       <c r="B53" s="7" t="n">
-        <v>5250</v>
+        <v>5200</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>10</v>
@@ -1764,19 +1815,19 @@
     </row>
     <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B54" s="7" t="n">
-        <v>5260</v>
+        <v>5210</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>10</v>
@@ -1784,19 +1835,19 @@
     </row>
     <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B55" s="7" t="n">
-        <v>5270</v>
+        <v>5220</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>10</v>
@@ -1804,19 +1855,19 @@
     </row>
     <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B56" s="7" t="n">
-        <v>5280</v>
+        <v>5230</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>10</v>
@@ -1824,19 +1875,19 @@
     </row>
     <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B57" s="7" t="n">
-        <v>5290</v>
+        <v>5240</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>10</v>
@@ -1844,19 +1895,19 @@
     </row>
     <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B58" s="7" t="n">
-        <v>5300</v>
+        <v>5250</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>10</v>
@@ -1864,19 +1915,19 @@
     </row>
     <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B59" s="7" t="n">
-        <v>5310</v>
+        <v>5260</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>10</v>
@@ -1884,19 +1935,19 @@
     </row>
     <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B60" s="7" t="n">
-        <v>5320</v>
+        <v>5270</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>10</v>
@@ -1904,19 +1955,19 @@
     </row>
     <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B61" s="7" t="n">
-        <v>5330</v>
+        <v>5280</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>10</v>
@@ -1924,19 +1975,19 @@
     </row>
     <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B62" s="7" t="n">
-        <v>5340</v>
+        <v>5290</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>10</v>
@@ -1944,19 +1995,19 @@
     </row>
     <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B63" s="7" t="n">
-        <v>5350</v>
+        <v>5300</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>10</v>
@@ -1964,19 +2015,19 @@
     </row>
     <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B64" s="7" t="n">
-        <v>5360</v>
+        <v>5310</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>10</v>
@@ -1984,19 +2035,19 @@
     </row>
     <row r="65" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B65" s="7" t="n">
-        <v>5370</v>
+        <v>5320</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>10</v>
@@ -2004,19 +2055,19 @@
     </row>
     <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B66" s="7" t="n">
-        <v>5380</v>
+        <v>5330</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>10</v>
@@ -2024,19 +2075,19 @@
     </row>
     <row r="67" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B67" s="7" t="n">
-        <v>5390</v>
+        <v>5340</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>10</v>
@@ -2044,19 +2095,19 @@
     </row>
     <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B68" s="7" t="n">
-        <v>5400</v>
+        <v>5350</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>10</v>
@@ -2064,19 +2115,19 @@
     </row>
     <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B69" s="7" t="n">
-        <v>5410</v>
+        <v>5360</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>10</v>
@@ -2084,19 +2135,19 @@
     </row>
     <row r="70" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B70" s="7" t="n">
-        <v>5420</v>
+        <v>5370</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>10</v>
@@ -2104,19 +2155,19 @@
     </row>
     <row r="71" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B71" s="7" t="n">
-        <v>5430</v>
+        <v>5380</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>10</v>
@@ -2124,19 +2175,19 @@
     </row>
     <row r="72" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B72" s="7" t="n">
-        <v>5440</v>
+        <v>5390</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>10</v>
@@ -2144,19 +2195,19 @@
     </row>
     <row r="73" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B73" s="7" t="n">
-        <v>5460</v>
+        <v>5400</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>10</v>
@@ -2164,19 +2215,19 @@
     </row>
     <row r="74" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B74" s="7" t="n">
-        <v>5470</v>
+        <v>5410</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>10</v>
@@ -2184,19 +2235,19 @@
     </row>
     <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B75" s="7" t="n">
-        <v>5480</v>
+        <v>5420</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>10</v>
@@ -2204,19 +2255,19 @@
     </row>
     <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B76" s="7" t="n">
-        <v>5600</v>
+        <v>5430</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>10</v>
@@ -2224,19 +2275,19 @@
     </row>
     <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B77" s="7" t="n">
-        <v>5800</v>
+        <v>5440</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>10</v>
@@ -2247,16 +2298,16 @@
         <v>106</v>
       </c>
       <c r="B78" s="7" t="n">
-        <v>5810</v>
+        <v>5460</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>10</v>
@@ -2267,58 +2318,158 @@
         <v>107</v>
       </c>
       <c r="B79" s="7" t="n">
-        <v>4200</v>
+        <v>5470</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B80" s="7" t="n">
-        <v>4210</v>
+        <v>5480</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B81" s="7" t="n">
+        <v>5600</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B81" s="7" t="n">
+      <c r="B82" s="7" t="n">
+        <v>5800</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B83" s="7" t="n">
+        <v>5810</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" s="7" t="n">
+        <v>4200</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B85" s="7" t="n">
+        <v>4210</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B86" s="7" t="n">
         <v>5900</v>
       </c>
-      <c r="C81" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F81" s="7" t="s">
+      <c r="C86" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2341,7 +2492,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="41:46 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2378,7 +2529,7 @@
     </row>
     <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1000</v>
@@ -2399,7 +2550,7 @@
     </row>
     <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1010</v>
@@ -2420,7 +2571,7 @@
     </row>
     <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>1020</v>
@@ -2441,7 +2592,7 @@
     </row>
     <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1030</v>
@@ -2462,7 +2613,7 @@
     </row>
     <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>1040</v>
@@ -2504,7 +2655,7 @@
     </row>
     <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>1210</v>
@@ -2576,7 +2727,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>24</v>
@@ -2597,7 +2748,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>24</v>
@@ -2618,7 +2769,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>24</v>
@@ -2639,7 +2790,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>24</v>
@@ -2660,7 +2811,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>24</v>
@@ -2681,7 +2832,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>24</v>
@@ -3197,7 +3348,7 @@
     </row>
     <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="B41" s="7" t="n">
         <v>4470</v>
@@ -3218,7 +3369,7 @@
     </row>
     <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B42" s="7" t="n">
         <v>4800</v>
@@ -3227,10 +3378,10 @@
         <v>52</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>10</v>
@@ -3239,7 +3390,7 @@
     </row>
     <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B43" s="7" t="n">
         <v>5000</v>
@@ -3248,19 +3399,19 @@
         <v>52</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="8"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B44" s="7" t="n">
         <v>5010</v>
@@ -3269,10 +3420,10 @@
         <v>52</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>10</v>
@@ -3280,7 +3431,7 @@
     </row>
     <row r="45" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B45" s="7" t="n">
         <v>5020</v>
@@ -3289,10 +3440,10 @@
         <v>52</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>10</v>
@@ -3300,7 +3451,7 @@
     </row>
     <row r="46" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B46" s="7" t="n">
         <v>5030</v>
@@ -3309,10 +3460,10 @@
         <v>52</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>10</v>
@@ -3320,7 +3471,7 @@
     </row>
     <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B47" s="7" t="n">
         <v>5040</v>
@@ -3329,10 +3480,10 @@
         <v>52</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>10</v>
@@ -3340,7 +3491,7 @@
     </row>
     <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B48" s="7" t="n">
         <v>5200</v>
@@ -3349,10 +3500,10 @@
         <v>52</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>10</v>
@@ -3360,7 +3511,7 @@
     </row>
     <row r="49" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B49" s="7" t="n">
         <v>5210</v>
@@ -3369,10 +3520,10 @@
         <v>52</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>10</v>
@@ -3380,7 +3531,7 @@
     </row>
     <row r="50" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B50" s="7" t="n">
         <v>5220</v>
@@ -3389,10 +3540,10 @@
         <v>52</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>10</v>
@@ -3400,7 +3551,7 @@
     </row>
     <row r="51" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B51" s="7" t="n">
         <v>5230</v>
@@ -3409,10 +3560,10 @@
         <v>52</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>10</v>
@@ -3420,7 +3571,7 @@
     </row>
     <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B52" s="7" t="n">
         <v>5240</v>
@@ -3429,10 +3580,10 @@
         <v>52</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>10</v>
@@ -3440,7 +3591,7 @@
     </row>
     <row r="53" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B53" s="7" t="n">
         <v>5250</v>
@@ -3449,10 +3600,10 @@
         <v>52</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>10</v>
@@ -3460,7 +3611,7 @@
     </row>
     <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B54" s="7" t="n">
         <v>5260</v>
@@ -3469,10 +3620,10 @@
         <v>52</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>10</v>
@@ -3480,7 +3631,7 @@
     </row>
     <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B55" s="7" t="n">
         <v>5270</v>
@@ -3489,10 +3640,10 @@
         <v>52</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>10</v>
@@ -3500,7 +3651,7 @@
     </row>
     <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B56" s="7" t="n">
         <v>5280</v>
@@ -3509,10 +3660,10 @@
         <v>52</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>10</v>
@@ -3520,7 +3671,7 @@
     </row>
     <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B57" s="7" t="n">
         <v>5290</v>
@@ -3529,10 +3680,10 @@
         <v>52</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>10</v>
@@ -3540,7 +3691,7 @@
     </row>
     <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B58" s="7" t="n">
         <v>5300</v>
@@ -3549,10 +3700,10 @@
         <v>52</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>10</v>
@@ -3560,7 +3711,7 @@
     </row>
     <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B59" s="7" t="n">
         <v>5310</v>
@@ -3569,10 +3720,10 @@
         <v>52</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F59" s="7" t="s">
         <v>10</v>
@@ -3580,7 +3731,7 @@
     </row>
     <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B60" s="7" t="n">
         <v>5320</v>
@@ -3589,10 +3740,10 @@
         <v>52</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F60" s="7" t="s">
         <v>10</v>
@@ -3600,7 +3751,7 @@
     </row>
     <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B61" s="7" t="n">
         <v>5330</v>
@@ -3609,10 +3760,10 @@
         <v>52</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>10</v>
@@ -3620,7 +3771,7 @@
     </row>
     <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B62" s="7" t="n">
         <v>5340</v>
@@ -3629,10 +3780,10 @@
         <v>52</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>10</v>
@@ -3640,7 +3791,7 @@
     </row>
     <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B63" s="7" t="n">
         <v>5350</v>
@@ -3649,10 +3800,10 @@
         <v>52</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F63" s="7" t="s">
         <v>10</v>
@@ -3660,7 +3811,7 @@
     </row>
     <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B64" s="7" t="n">
         <v>5360</v>
@@ -3669,10 +3820,10 @@
         <v>52</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>10</v>
@@ -3680,7 +3831,7 @@
     </row>
     <row r="65" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B65" s="7" t="n">
         <v>5370</v>
@@ -3689,10 +3840,10 @@
         <v>52</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F65" s="7" t="s">
         <v>10</v>
@@ -3700,7 +3851,7 @@
     </row>
     <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B66" s="7" t="n">
         <v>5380</v>
@@ -3709,10 +3860,10 @@
         <v>52</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>10</v>
@@ -3720,7 +3871,7 @@
     </row>
     <row r="67" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B67" s="7" t="n">
         <v>5390</v>
@@ -3729,10 +3880,10 @@
         <v>52</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>10</v>
@@ -3740,7 +3891,7 @@
     </row>
     <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B68" s="7" t="n">
         <v>5400</v>
@@ -3749,10 +3900,10 @@
         <v>52</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>10</v>
@@ -3760,7 +3911,7 @@
     </row>
     <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B69" s="7" t="n">
         <v>5410</v>
@@ -3769,10 +3920,10 @@
         <v>52</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>10</v>
@@ -3780,7 +3931,7 @@
     </row>
     <row r="70" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B70" s="7" t="n">
         <v>5420</v>
@@ -3789,10 +3940,10 @@
         <v>52</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>10</v>
@@ -3800,7 +3951,7 @@
     </row>
     <row r="71" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B71" s="7" t="n">
         <v>5430</v>
@@ -3809,10 +3960,10 @@
         <v>52</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>10</v>
@@ -3820,7 +3971,7 @@
     </row>
     <row r="72" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B72" s="7" t="n">
         <v>5440</v>
@@ -3829,10 +3980,10 @@
         <v>52</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F72" s="7" t="s">
         <v>10</v>
@@ -3840,7 +3991,7 @@
     </row>
     <row r="73" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B73" s="7" t="n">
         <v>5450</v>
@@ -3849,10 +4000,10 @@
         <v>52</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F73" s="7" t="s">
         <v>10</v>
@@ -3860,7 +4011,7 @@
     </row>
     <row r="74" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B74" s="7" t="n">
         <v>5460</v>
@@ -3869,10 +4020,10 @@
         <v>52</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>10</v>
@@ -3880,7 +4031,7 @@
     </row>
     <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B75" s="7" t="n">
         <v>5470</v>
@@ -3889,10 +4040,10 @@
         <v>52</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>10</v>
@@ -3900,7 +4051,7 @@
     </row>
     <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B76" s="7" t="n">
         <v>5480</v>
@@ -3909,10 +4060,10 @@
         <v>52</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>10</v>
@@ -3920,7 +4071,7 @@
     </row>
     <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B77" s="7" t="n">
         <v>5600</v>
@@ -3929,10 +4080,10 @@
         <v>52</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>10</v>
@@ -3940,7 +4091,7 @@
     </row>
     <row r="78" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B78" s="7" t="n">
         <v>5800</v>
@@ -3949,10 +4100,10 @@
         <v>52</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>10</v>
@@ -3960,7 +4111,7 @@
     </row>
     <row r="79" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B79" s="7" t="n">
         <v>5810</v>
@@ -3969,10 +4120,10 @@
         <v>52</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>10</v>
@@ -3980,7 +4131,7 @@
     </row>
     <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B80" s="7" t="n">
         <v>4200</v>
@@ -3992,7 +4143,7 @@
         <v>53</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>17</v>
@@ -4000,7 +4151,7 @@
     </row>
     <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B81" s="7" t="n">
         <v>4210</v>
@@ -4012,7 +4163,7 @@
         <v>53</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>17</v>
@@ -4020,7 +4171,7 @@
     </row>
     <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B82" s="7" t="n">
         <v>5900</v>
@@ -4029,10 +4180,10 @@
         <v>52</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>10</v>

</xml_diff>